<commit_message>
Fixed up incorrect import code, closes #232
</commit_message>
<xml_diff>
--- a/tests/data/import.xlsx
+++ b/tests/data/import.xlsx
@@ -18,49 +18,49 @@
     <t>Do not modify the first row in every sheet!</t>
   </si>
   <si>
+    <t>assignment:media_items</t>
+  </si>
+  <si>
     <t>participant_experiment:experiment</t>
   </si>
   <si>
-    <t>assignment:media_items</t>
+    <t>Simply add in your data in the rows undeneath it.</t>
+  </si>
+  <si>
+    <t>Use IDs from the export sheet to populate relationship columns.</t>
+  </si>
+  <si>
+    <t>If you want multiple objects in a relation, separate the IDs using commas.</t>
+  </si>
+  <si>
+    <t>There is no need to modify any sheet if you are not interested in adding in objects of that type</t>
+  </si>
+  <si>
+    <t>Example: To make an experiment and use existing assignments for the experiment, fill out the Experiments, Participant Experiment, and Assignment sheets.</t>
+  </si>
+  <si>
+    <t>Example: To add assignments to an existing experiment, fill out the Participant Experiment and Assignment sheet. For the participant_experiment_experiment column, use the experiment_id of the experiment you wish to modify. You can find this ID in the export spreadsheet.</t>
+  </si>
+  <si>
+    <t>If you wish to do one the above as well as create new activities, fill out the sheets mentioned above as well as the Activities sheet. If you are making new multiple choice questions, you'll also need to fill out the Choices sheet.</t>
   </si>
   <si>
     <t>participant_experiment:assignments</t>
   </si>
   <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>5,6</t>
+  </si>
+  <si>
     <t>assignment:activity</t>
   </si>
   <si>
-    <t>Simply add in your data in the rows undeneath it.</t>
-  </si>
-  <si>
     <t>assignment:id</t>
-  </si>
-  <si>
-    <t>Use IDs from the export sheet to populate relationship columns.</t>
-  </si>
-  <si>
-    <t>If you want multiple objects in a relation, separate the IDs using commas.</t>
-  </si>
-  <si>
-    <t>There is no need to modify any sheet if you are not interested in adding in objects of that type</t>
-  </si>
-  <si>
-    <t>Example: To make an experiment and use existing assignments for the experiment, fill out the Experiments, Participant Experiment, and Assignment sheets.</t>
-  </si>
-  <si>
-    <t>Example: To add assignments to an existing experiment, fill out the Participant Experiment and Assignment sheet. For the participant_experiment_experiment column, use the experiment_id of the experiment you wish to modify. You can find this ID in the export spreadsheet.</t>
-  </si>
-  <si>
-    <t>If you wish to do one the above as well as create new activities, fill out the sheets mentioned above as well as the Activities sheet. If you are making new multiple choice questions, you'll also need to fill out the Choices sheet.</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>2,1</t>
-  </si>
-  <si>
-    <t>1,3</t>
   </si>
 </sst>
 </file>
@@ -139,37 +139,37 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -191,13 +191,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
@@ -213,7 +213,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B3" s="2">
         <v>2.0</v>
@@ -224,7 +224,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B4" s="2">
         <v>3.0</v>
@@ -232,6 +232,45 @@
       <c r="C4" s="2">
         <v>3.0</v>
       </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="C9" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -245,15 +284,16 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="9.38"/>
+    <col customWidth="1" min="1" max="1" width="24.13"/>
+    <col customWidth="1" min="2" max="26" width="9.38"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -261,7 +301,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -269,7 +309,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -277,7 +317,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>